<commit_message>
Preparing for initial deployment
</commit_message>
<xml_diff>
--- a/bid checklist.xlsx
+++ b/bid checklist.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/willstrader/Desktop/API-Projects/scherrer-ai-agent/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{014F5FF1-5798-234B-8AA7-CC068DE2196A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{11F74508-606D-A24D-9EFB-1786E3E4950A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="740" windowWidth="30240" windowHeight="18900" xr2:uid="{BE96ED08-D6E4-424B-ADF9-265457548A6A}"/>
   </bookViews>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="33">
   <si>
     <t>Permit cost by who?</t>
   </si>
@@ -53,9 +53,6 @@
   </si>
   <si>
     <t>Start date</t>
-  </si>
-  <si>
-    <t>Which trades?</t>
   </si>
   <si>
     <t>Testing by who?</t>
@@ -74,23 +71,6 @@
     <t>Insurance requirements beyond typical</t>
   </si>
   <si>
-    <r>
-      <t xml:space="preserve">If yes </t>
-    </r>
-    <r>
-      <rPr>
-        <u/>
-        <sz val="10"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>  $                /DAY</t>
-    </r>
-  </si>
-  <si>
-    <t>Liquated Damages?</t>
-  </si>
-  <si>
     <t>SBE/DBE/TBE required?</t>
   </si>
   <si>
@@ -128,9 +108,6 @@
     <t>Signature by who?</t>
   </si>
   <si>
-    <t>How Many?</t>
-  </si>
-  <si>
     <r>
       <rPr>
         <sz val="10"/>
@@ -195,25 +172,6 @@
         <rFont val="Calibri"/>
         <family val="2"/>
       </rPr>
-      <t xml:space="preserve">AIA Form </t>
-    </r>
-    <r>
-      <rPr>
-        <u/>
-        <sz val="10"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>                                </t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
       <t>Pre-Qualification?</t>
     </r>
   </si>
@@ -226,9 +184,6 @@
       </rPr>
       <t>Pre-Bid Mandatory?</t>
     </r>
-  </si>
-  <si>
-    <t>Date, Time, Location:</t>
   </si>
   <si>
     <t>Pre-Bid Conference
@@ -238,9 +193,6 @@
     <t>Peformance Bond Required?</t>
   </si>
   <si>
-    <t>5 or 10%</t>
-  </si>
-  <si>
     <r>
       <rPr>
         <sz val="10"/>
@@ -259,12 +211,6 @@
       </rPr>
       <t>Public Opening?</t>
     </r>
-  </si>
-  <si>
-    <t>Bid turn online</t>
-  </si>
-  <si>
-    <t>Bid turn in in person</t>
   </si>
   <si>
     <r>
@@ -321,13 +267,19 @@
   </si>
   <si>
     <t>Answer</t>
+  </si>
+  <si>
+    <t>Liquidated Damages?</t>
+  </si>
+  <si>
+    <t>Bid turn in in person or online</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -348,12 +300,6 @@
     </font>
     <font>
       <b/>
-      <sz val="10"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <u/>
       <sz val="10"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -672,7 +618,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="48">
+  <cellXfs count="47">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
@@ -707,7 +653,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="1" applyBorder="1" applyAlignment="1">
@@ -734,7 +680,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="1" applyBorder="1" applyAlignment="1">
@@ -758,7 +704,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="12" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -770,7 +716,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="16" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="16" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -785,13 +731,13 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="21" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="22" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="22" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="18" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="18" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -800,12 +746,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -813,6 +753,9 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1120,15 +1063,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BF83CAB1-2421-4680-996F-846E3D70DF7F}">
-  <dimension ref="A1:N34"/>
+  <dimension ref="A1:N33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
-      <selection activeCell="J27" sqref="J27:N27"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="J19" sqref="J19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="13" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="18.83203125" style="1" customWidth="1"/>
+    <col min="1" max="1" width="21.5" style="1" customWidth="1"/>
     <col min="2" max="2" width="7.1640625" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10.83203125" style="1" customWidth="1"/>
     <col min="4" max="4" width="5.83203125" style="1" customWidth="1"/>
@@ -1139,7 +1082,7 @@
   <sheetData>
     <row r="1" spans="1:6" ht="21.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1" s="38" t="s">
-        <v>38</v>
+        <v>29</v>
       </c>
       <c r="B1" s="37"/>
       <c r="C1" s="37"/>
@@ -1149,7 +1092,7 @@
     </row>
     <row r="2" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="35" t="s">
-        <v>37</v>
+        <v>28</v>
       </c>
       <c r="B2" s="39"/>
       <c r="C2" s="39"/>
@@ -1159,7 +1102,7 @@
     </row>
     <row r="3" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="35" t="s">
-        <v>36</v>
+        <v>27</v>
       </c>
       <c r="B3" s="39"/>
       <c r="C3" s="39"/>
@@ -1169,7 +1112,7 @@
     </row>
     <row r="4" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="35" t="s">
-        <v>35</v>
+        <v>26</v>
       </c>
       <c r="B4" s="39"/>
       <c r="C4" s="39"/>
@@ -1179,7 +1122,7 @@
     </row>
     <row r="5" spans="1:6" ht="30" x14ac:dyDescent="0.15">
       <c r="A5" s="35" t="s">
-        <v>34</v>
+        <v>25</v>
       </c>
       <c r="B5" s="39"/>
       <c r="C5" s="39"/>
@@ -1190,7 +1133,7 @@
     <row r="6" spans="1:6" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A6" s="34"/>
       <c r="B6" s="33" t="s">
-        <v>39</v>
+        <v>30</v>
       </c>
       <c r="C6" s="32"/>
       <c r="D6" s="32"/>
@@ -1199,7 +1142,7 @@
     </row>
     <row r="7" spans="1:6" ht="15" x14ac:dyDescent="0.15">
       <c r="A7" s="30" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B7" s="29"/>
       <c r="C7" s="28"/>
@@ -1207,85 +1150,78 @@
       <c r="E7" s="28"/>
       <c r="F7" s="27"/>
     </row>
-    <row r="8" spans="1:6" ht="15" x14ac:dyDescent="0.15">
-      <c r="A8" s="30" t="s">
-        <v>32</v>
-      </c>
-      <c r="B8" s="29"/>
-      <c r="C8" s="28"/>
-      <c r="D8" s="28"/>
-      <c r="E8" s="28"/>
-      <c r="F8" s="27"/>
-    </row>
-    <row r="9" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="B8" s="23"/>
+      <c r="C8" s="19"/>
+      <c r="D8" s="19"/>
+      <c r="E8" s="19"/>
+      <c r="F8" s="18"/>
+    </row>
+    <row r="9" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="9" t="s">
-        <v>31</v>
+        <v>23</v>
       </c>
       <c r="B9" s="23"/>
       <c r="C9" s="19"/>
-      <c r="D9" s="19"/>
-      <c r="E9" s="19"/>
-      <c r="F9" s="18"/>
-    </row>
-    <row r="10" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="D9" s="20"/>
+      <c r="E9" s="20"/>
+      <c r="F9" s="22"/>
+    </row>
+    <row r="10" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="9" t="s">
-        <v>30</v>
+        <v>22</v>
       </c>
       <c r="B10" s="23"/>
-      <c r="C10" s="19" t="s">
-        <v>29</v>
-      </c>
+      <c r="C10" s="19"/>
       <c r="D10" s="20"/>
       <c r="E10" s="20"/>
       <c r="F10" s="22"/>
     </row>
     <row r="11" spans="1:6" ht="30" x14ac:dyDescent="0.2">
       <c r="A11" s="9" t="s">
-        <v>28</v>
-      </c>
-      <c r="B11" s="23"/>
+        <v>21</v>
+      </c>
+      <c r="B11" s="21"/>
       <c r="C11" s="19"/>
       <c r="D11" s="20"/>
       <c r="E11" s="20"/>
       <c r="F11" s="22"/>
     </row>
-    <row r="12" spans="1:6" ht="30" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="9" t="s">
-        <v>27</v>
-      </c>
-      <c r="B12" s="21"/>
-      <c r="C12" s="19" t="s">
-        <v>26</v>
-      </c>
-      <c r="D12" s="20"/>
-      <c r="E12" s="20"/>
-      <c r="F12" s="22"/>
+        <v>20</v>
+      </c>
+      <c r="B12" s="23"/>
+      <c r="C12" s="19"/>
+      <c r="D12" s="19"/>
+      <c r="E12" s="19"/>
+      <c r="F12" s="18"/>
     </row>
     <row r="13" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="9" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="B13" s="23"/>
       <c r="C13" s="19"/>
-      <c r="D13" s="19"/>
-      <c r="E13" s="19"/>
-      <c r="F13" s="18"/>
-    </row>
-    <row r="14" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="9" t="s">
-        <v>24</v>
-      </c>
-      <c r="B14" s="23"/>
-      <c r="C14" s="19"/>
-      <c r="D14" s="41" t="s">
-        <v>23</v>
-      </c>
-      <c r="E14" s="41"/>
-      <c r="F14" s="42"/>
+      <c r="E13" s="41"/>
+      <c r="F13" s="42"/>
+    </row>
+    <row r="14" spans="1:6" ht="40" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A14" s="13" t="s">
+        <v>18</v>
+      </c>
+      <c r="B14" s="26"/>
+      <c r="C14" s="25"/>
+      <c r="D14" s="41"/>
+      <c r="E14" s="25"/>
+      <c r="F14" s="24"/>
     </row>
     <row r="15" spans="1:6" ht="30" x14ac:dyDescent="0.2">
       <c r="A15" s="13" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="B15" s="26"/>
       <c r="C15" s="25"/>
@@ -1293,93 +1229,89 @@
       <c r="E15" s="25"/>
       <c r="F15" s="24"/>
     </row>
-    <row r="16" spans="1:6" ht="30" x14ac:dyDescent="0.2">
-      <c r="A16" s="13" t="s">
-        <v>21</v>
-      </c>
-      <c r="B16" s="26"/>
-      <c r="C16" s="25"/>
-      <c r="D16" s="25"/>
-      <c r="E16" s="25"/>
-      <c r="F16" s="24"/>
+    <row r="16" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A16" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="B16" s="23"/>
+      <c r="C16" s="19"/>
+      <c r="D16" s="19"/>
+      <c r="E16" s="19"/>
+      <c r="F16" s="18"/>
     </row>
     <row r="17" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="9" t="s">
-        <v>20</v>
-      </c>
-      <c r="B17" s="23"/>
-      <c r="C17" s="19" t="s">
-        <v>18</v>
-      </c>
-      <c r="D17" s="19"/>
-      <c r="E17" s="19"/>
-      <c r="F17" s="18"/>
-    </row>
-    <row r="18" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+        <v>15</v>
+      </c>
+      <c r="B17" s="21"/>
+      <c r="C17" s="19"/>
+      <c r="D17" s="20"/>
+      <c r="E17" s="20"/>
+      <c r="F17" s="22"/>
+    </row>
+    <row r="18" spans="1:14" ht="15" x14ac:dyDescent="0.2">
       <c r="A18" s="9" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="B18" s="21"/>
-      <c r="C18" s="19" t="s">
-        <v>18</v>
-      </c>
-      <c r="D18" s="20"/>
-      <c r="E18" s="20"/>
-      <c r="F18" s="22"/>
-    </row>
-    <row r="19" spans="1:14" ht="15" x14ac:dyDescent="0.2">
+      <c r="C18" s="20"/>
+      <c r="D18" s="19"/>
+      <c r="E18" s="19"/>
+      <c r="F18" s="18"/>
+    </row>
+    <row r="19" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A19" s="9" t="s">
-        <v>17</v>
-      </c>
-      <c r="B19" s="21"/>
-      <c r="C19" s="20"/>
-      <c r="D19" s="19"/>
-      <c r="E19" s="19"/>
-      <c r="F19" s="18"/>
-    </row>
-    <row r="20" spans="1:14" ht="30" x14ac:dyDescent="0.15">
+        <v>13</v>
+      </c>
+      <c r="B19" s="8"/>
+      <c r="C19" s="7"/>
+      <c r="D19" s="7"/>
+      <c r="E19" s="17"/>
+      <c r="F19" s="16"/>
+    </row>
+    <row r="20" spans="1:14" ht="15" x14ac:dyDescent="0.15">
       <c r="A20" s="9" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="B20" s="8"/>
-      <c r="C20" s="43"/>
-      <c r="D20" s="43"/>
+      <c r="C20" s="7"/>
+      <c r="D20" s="7"/>
       <c r="E20" s="17"/>
       <c r="F20" s="16"/>
     </row>
-    <row r="21" spans="1:14" ht="15" x14ac:dyDescent="0.15">
+    <row r="21" spans="1:14" ht="30" x14ac:dyDescent="0.2">
       <c r="A21" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="B21" s="8"/>
-      <c r="C21" s="7"/>
-      <c r="D21" s="7"/>
-      <c r="E21" s="17"/>
-      <c r="F21" s="16"/>
+        <v>11</v>
+      </c>
+      <c r="B21" s="12"/>
+      <c r="C21" s="43"/>
+      <c r="D21" s="43"/>
+      <c r="E21" s="15"/>
+      <c r="F21" s="14"/>
     </row>
     <row r="22" spans="1:14" ht="30" x14ac:dyDescent="0.2">
-      <c r="A22" s="9" t="s">
-        <v>14</v>
+      <c r="A22" s="13" t="s">
+        <v>10</v>
       </c>
       <c r="B22" s="12"/>
-      <c r="C22" s="45"/>
-      <c r="D22" s="45"/>
-      <c r="E22" s="15"/>
-      <c r="F22" s="14"/>
-    </row>
-    <row r="23" spans="1:14" ht="30" x14ac:dyDescent="0.2">
-      <c r="A23" s="13" t="s">
-        <v>13</v>
-      </c>
-      <c r="B23" s="12"/>
-      <c r="C23" s="46"/>
-      <c r="D23" s="46"/>
-      <c r="E23" s="11"/>
-      <c r="F23" s="10"/>
+      <c r="C22" s="44"/>
+      <c r="D22" s="44"/>
+      <c r="E22" s="11"/>
+      <c r="F22" s="10"/>
+    </row>
+    <row r="23" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A23" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="B23" s="8"/>
+      <c r="C23" s="7"/>
+      <c r="D23" s="7"/>
+      <c r="E23" s="7"/>
+      <c r="F23" s="6"/>
     </row>
     <row r="24" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="9" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="B24" s="8"/>
       <c r="C24" s="7"/>
@@ -1387,46 +1319,44 @@
       <c r="E24" s="7"/>
       <c r="F24" s="6"/>
     </row>
-    <row r="25" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:14" ht="15" x14ac:dyDescent="0.2">
       <c r="A25" s="9" t="s">
-        <v>11</v>
+        <v>31</v>
       </c>
       <c r="B25" s="8"/>
       <c r="C25" s="7"/>
-      <c r="D25" s="7"/>
-      <c r="E25" s="7"/>
+      <c r="D25" s="43"/>
+      <c r="E25" s="45"/>
       <c r="F25" s="6"/>
     </row>
-    <row r="26" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:14" ht="30" x14ac:dyDescent="0.2">
       <c r="A26" s="9" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="B26" s="8"/>
-      <c r="C26" s="43" t="s">
-        <v>9</v>
-      </c>
-      <c r="D26" s="45"/>
-      <c r="E26" s="47"/>
+      <c r="C26" s="7"/>
+      <c r="D26" s="7"/>
+      <c r="E26" s="7"/>
       <c r="F26" s="6"/>
-    </row>
-    <row r="27" spans="1:14" ht="133.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="J26" s="46"/>
+      <c r="K26" s="46"/>
+      <c r="L26" s="46"/>
+      <c r="M26" s="46"/>
+      <c r="N26" s="46"/>
+    </row>
+    <row r="27" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" s="9" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B27" s="8"/>
       <c r="C27" s="7"/>
       <c r="D27" s="7"/>
       <c r="E27" s="7"/>
       <c r="F27" s="6"/>
-      <c r="J27" s="44"/>
-      <c r="K27" s="44"/>
-      <c r="L27" s="44"/>
-      <c r="M27" s="44"/>
-      <c r="N27" s="44"/>
-    </row>
-    <row r="28" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="28" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="9" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B28" s="8"/>
       <c r="C28" s="7"/>
@@ -1434,9 +1364,9 @@
       <c r="E28" s="7"/>
       <c r="F28" s="6"/>
     </row>
-    <row r="29" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:14" ht="27" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" s="9" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B29" s="8"/>
       <c r="C29" s="7"/>
@@ -1444,9 +1374,9 @@
       <c r="E29" s="7"/>
       <c r="F29" s="6"/>
     </row>
-    <row r="30" spans="1:14" ht="27" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:14" ht="38.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" s="9" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B30" s="8"/>
       <c r="C30" s="7"/>
@@ -1454,21 +1384,19 @@
       <c r="E30" s="7"/>
       <c r="F30" s="6"/>
     </row>
-    <row r="31" spans="1:14" ht="38.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A31" s="9" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B31" s="8"/>
-      <c r="C31" s="7" t="s">
-        <v>3</v>
-      </c>
+      <c r="C31" s="7"/>
       <c r="D31" s="7"/>
       <c r="E31" s="7"/>
       <c r="F31" s="6"/>
     </row>
     <row r="32" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A32" s="9" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B32" s="8"/>
       <c r="C32" s="7"/>
@@ -1476,38 +1404,19 @@
       <c r="E32" s="7"/>
       <c r="F32" s="6"/>
     </row>
-    <row r="33" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A33" s="9" t="s">
-        <v>1</v>
-      </c>
-      <c r="B33" s="8"/>
-      <c r="C33" s="7"/>
-      <c r="D33" s="7"/>
-      <c r="E33" s="7"/>
-      <c r="F33" s="6"/>
-    </row>
-    <row r="34" spans="1:6" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="5" t="s">
+    <row r="33" spans="1:6" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A33" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B34" s="4"/>
-      <c r="C34" s="3"/>
-      <c r="D34" s="3"/>
-      <c r="E34" s="3"/>
-      <c r="F34" s="2"/>
+      <c r="B33" s="4"/>
+      <c r="C33" s="3"/>
+      <c r="D33" s="3"/>
+      <c r="E33" s="3"/>
+      <c r="F33" s="2"/>
     </row>
   </sheetData>
-  <mergeCells count="10">
-    <mergeCell ref="B2:F2"/>
-    <mergeCell ref="B3:F3"/>
-    <mergeCell ref="D14:F14"/>
-    <mergeCell ref="C20:D20"/>
-    <mergeCell ref="J27:N27"/>
-    <mergeCell ref="C22:D22"/>
-    <mergeCell ref="C23:D23"/>
-    <mergeCell ref="C26:E26"/>
-    <mergeCell ref="B5:F5"/>
-    <mergeCell ref="B4:F4"/>
+  <mergeCells count="1">
+    <mergeCell ref="J26:N26"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>